<commit_message>
ACCURATE CALCULATIONS !! :D
</commit_message>
<xml_diff>
--- a/Exports/Results1.xlsx
+++ b/Exports/Results1.xlsx
@@ -566,7 +566,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.0980070444692341</t>
+          <t>0.999999715665001</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.307833817193853</t>
+          <t>0.879140052591499</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.842136885478279</t>
+          <t>0.995088226113807</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.174895871268657</t>
+          <t>0.994500027996446</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.251310395873227</t>
+          <t>0.999766160128656</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.0028437517390715</t>
+          <t>0.999724347062487</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -938,7 +938,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.639778895349795</t>
+          <t>0.867173527352789</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0.791656029003398</t>
+          <t>0.999449251287372</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0.000227286312765886</t>
+          <t>0.000258409368966036</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>1080.88278898945</t>
+          <t>1228.89159505488</t>
         </is>
       </c>
     </row>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.0503863013198322</t>
+          <t>0.97705864973909</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.228163792757875</t>
+          <t>0.936265166036628</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.167800061728358</t>
+          <t>0.999687578373293</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.193807106958561</t>
+          <t>0.994676205886985</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.669662318487841</t>
+          <t>0.998331913118766</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1749,7 +1749,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0.473808197343776</t>
+          <t>0.995242587915354</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0.000240029533580422</t>
+          <t>0.000307410279866116</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1779,7 +1779,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2114.64098848083</t>
+          <t>2708.25997279809</t>
         </is>
       </c>
     </row>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0.405061075321775</t>
+          <t>0.998067649401291</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.16027135889666</t>
+          <t>0.920346057176682</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2240,7 +2240,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0.143961113456213</t>
+          <t>0.889412740332115</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2302,7 +2302,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.000467175424951053</t>
+          <t>0.958427942433311</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.082756174636248</t>
+          <t>0.927842354321809</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.486712418390757</t>
+          <t>0.90451852803558</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2612,7 +2612,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.352052672958662</t>
+          <t>0.987023914145289</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0.0525587938156666</t>
+          <t>0.969797598368199</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0.40508146938625</t>
+          <t>0.999327048148483</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.524028486315866</t>
+          <t>0.921502233691681</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2860,7 +2860,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0.711238460281365</t>
+          <t>0.94920801306659</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2922,7 +2922,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0.358601729954345</t>
+          <t>0.977856249753898</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2984,7 +2984,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.0904672935168706</t>
+          <t>0.987107167321343</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3046,12 +3046,12 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0.639747920730119</t>
+          <t>0.974689176594734</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0.0519558094475671</t>
+          <t>0.999735693644705</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>-3.28481823612768e-05</t>
+          <t>0.000138994748652222</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>-349.651820180964</t>
+          <t>1479.52682213361</t>
         </is>
       </c>
     </row>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.0529020907746822</t>
+          <t>0.898996779633501</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>0.0481788392294712</t>
+          <t>0.999641647347348</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -3319,7 +3319,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>3.80912108840266e-05</t>
+          <t>0.000245417552853434</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>410.946266798104</t>
+          <t>2647.68236060822</t>
         </is>
       </c>
     </row>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.73235880149322</t>
+          <t>0.945430671093185</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">

</xml_diff>